<commit_message>
Latest numbers with medium system included
</commit_message>
<xml_diff>
--- a/papers/impact_data/IMPACTsmallsystem.xlsx
+++ b/papers/impact_data/IMPACTsmallsystem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1140" windowWidth="23760" windowHeight="13220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Size of BJ</t>
   </si>
@@ -47,12 +47,15 @@
   <si>
     <t>Time per 10K</t>
   </si>
+  <si>
+    <t>Time per 25K</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,6 +87,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -102,7 +120,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -114,22 +132,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -250,11 +326,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2072491480"/>
-        <c:axId val="2063640200"/>
+        <c:axId val="2065419736"/>
+        <c:axId val="2070958344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2072491480"/>
+        <c:axId val="2065419736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -283,7 +359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063640200"/>
+        <c:crossAx val="2070958344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -291,7 +367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2063640200"/>
+        <c:axId val="2070958344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -321,7 +397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072491480"/>
+        <c:crossAx val="2065419736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -451,11 +527,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2063374408"/>
-        <c:axId val="2071280872"/>
+        <c:axId val="2056208904"/>
+        <c:axId val="2071329416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2063374408"/>
+        <c:axId val="2056208904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2071280872"/>
+        <c:crossAx val="2071329416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -492,7 +568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2071280872"/>
+        <c:axId val="2071329416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,7 +598,358 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063374408"/>
+        <c:crossAx val="2056208904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$11:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1008.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>336.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>168.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$11:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3821.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3095.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2373.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1145.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3152.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2068823032"/>
+        <c:axId val="2066999992"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2068823032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2066999992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2066999992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068823032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>IMPACT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> Medium System</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>Fixed BJ 504 Cores</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>Wall Clock Time to do 25K Steps</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$11:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$11:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.716666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.166666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.266666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.070833333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.983333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2068459336"/>
+        <c:axId val="2062982024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2068459336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Subjob</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Cores</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2062982024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2062982024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2068459336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -573,16 +1000,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -596,6 +1023,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -926,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1156,6 +1643,185 @@
         <v>0.6333333333333333</v>
       </c>
     </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>504</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>1008</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>72</v>
+      </c>
+      <c r="F11">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>3821</v>
+      </c>
+      <c r="H11">
+        <f>G11*25000*((1.5)*10^-6)/(1/24)</f>
+        <v>3438.9</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5.7166666670000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>504</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>336</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>3095</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H15" si="1">G12*25000*(1.5*10^-6)*1*24</f>
+        <v>2785.5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2.1666666669999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>504</v>
+      </c>
+      <c r="B13">
+        <v>60</v>
+      </c>
+      <c r="C13">
+        <v>168</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>2373</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2135.6999999999998</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.266666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>504</v>
+      </c>
+      <c r="B14">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>112</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>1145</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1030.5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.0708333329999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>504</v>
+      </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>84</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>3152</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>2836.8</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.98333333300000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Change table to nanoseconds per day
</commit_message>
<xml_diff>
--- a/papers/impact_data/IMPACTsmallsystem.xlsx
+++ b/papers/impact_data/IMPACTsmallsystem.xlsx
@@ -120,8 +120,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,7 +169,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -187,6 +189,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -206,6 +209,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -326,11 +330,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2065419736"/>
-        <c:axId val="2070958344"/>
+        <c:axId val="2067146984"/>
+        <c:axId val="2067406296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2065419736"/>
+        <c:axId val="2067146984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +363,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070958344"/>
+        <c:crossAx val="2067406296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -367,7 +371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2070958344"/>
+        <c:axId val="2067406296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065419736"/>
+        <c:crossAx val="2067146984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -527,11 +531,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2056208904"/>
-        <c:axId val="2071329416"/>
+        <c:axId val="2072325624"/>
+        <c:axId val="2072480744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2056208904"/>
+        <c:axId val="2072325624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2071329416"/>
+        <c:crossAx val="2072480744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -568,7 +572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2071329416"/>
+        <c:axId val="2072480744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,7 +602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056208904"/>
+        <c:crossAx val="2072325624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -701,11 +705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2068823032"/>
-        <c:axId val="2066999992"/>
+        <c:axId val="2063302616"/>
+        <c:axId val="2072669784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2068823032"/>
+        <c:axId val="2063302616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,12 +719,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066999992"/>
+        <c:crossAx val="2072669784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2066999992"/>
+        <c:axId val="2072669784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,7 +735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2068823032"/>
+        <c:crossAx val="2063302616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -873,11 +877,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2068459336"/>
-        <c:axId val="2062982024"/>
+        <c:axId val="2071839928"/>
+        <c:axId val="2071019080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2068459336"/>
+        <c:axId val="2071839928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +915,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062982024"/>
+        <c:crossAx val="2071019080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -919,7 +923,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2062982024"/>
+        <c:axId val="2071019080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,7 +953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2068459336"/>
+        <c:crossAx val="2071839928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1413,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1822,6 +1826,36 @@
         <v>0.98333333300000003</v>
       </c>
     </row>
+    <row r="17" spans="9:9">
+      <c r="I17">
+        <f>I11*60</f>
+        <v>343.00000002000002</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9">
+      <c r="I18">
+        <f t="shared" ref="I18:I21" si="2">I12*60</f>
+        <v>130.00000001999999</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9">
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>76.000000020000002</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9">
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>64.249999979999998</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9">
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>58.999999979999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>